<commit_message>
Added new example PD, small clean up on coefficient Excel
</commit_message>
<xml_diff>
--- a/antoinesCoefficients.xlsx
+++ b/antoinesCoefficients.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MATLAB\phaseDiagram\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\MATLAB\phaseDiagramTVL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34C90D06-BFE2-4E35-A776-8606CEB9CDAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9974C92B-1BF9-44D6-8C76-06B348C096FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16260" yWindow="8910" windowWidth="14670" windowHeight="8415" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27720" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -811,13 +811,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F147"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>